<commit_message>
Added total avg tto exel
</commit_message>
<xml_diff>
--- a/exel.xlsx
+++ b/exel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Google Drive\Tareas\Patos\proyecto\daily_temp_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iggym\Documents\Procesamiento Masivo de Datos\Project\daily_temp_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CB782A-881C-4069-A550-D23DDED3DEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBEEF94-7CFF-4F0B-9934-06755C8BB4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2580" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{EB65F998-C7A7-4408-AC65-F4F555A00757}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{EB65F998-C7A7-4408-AC65-F4F555A00757}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Spring</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>South/Central America &amp; Carribean</t>
+  </si>
+  <si>
+    <t>Avg total</t>
   </si>
 </sst>
 </file>
@@ -3526,10 +3529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C714A26-8582-4DED-B929-AA40AE456B7C}">
-  <dimension ref="E5:R32"/>
+  <dimension ref="D5:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,7 +3541,10 @@
     <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
@@ -3567,7 +3573,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>SUM(F6:I6)/4</f>
+        <v>63.956590158972574</v>
+      </c>
       <c r="E6">
         <v>1995</v>
       </c>
@@ -3586,7 +3596,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" ref="D7:D30" si="0">SUM(F7:I7)/4</f>
+        <v>63.045467870364796</v>
+      </c>
       <c r="E7">
         <v>1996</v>
       </c>
@@ -3607,19 +3621,23 @@
         <v>-0.92082935909429864</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ref="K7:M22" si="0">G7-G6</f>
+        <f t="shared" ref="K7:M22" si="1">G7-G6</f>
         <v>-0.81240918143539886</v>
       </c>
       <c r="L7" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.3093035265379029</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.60194708736349867</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>-1.3093035265379029</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.60194708736349867</v>
-      </c>
-    </row>
-    <row r="8" spans="5:13" x14ac:dyDescent="0.25">
+        <v>63.402785370641247</v>
+      </c>
       <c r="E8">
         <v>1997</v>
       </c>
@@ -3636,23 +3654,27 @@
         <v>60.182247880209196</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" ref="J8:J30" si="1">F8-F7</f>
+        <f t="shared" ref="J8:J30" si="2">F8-F7</f>
         <v>0.38041909702180021</v>
       </c>
       <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.14267765052549919</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.48570475346590314</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.70582380114359466</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>-0.14267765052549919</v>
-      </c>
-      <c r="L8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48570475346590314</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.70582380114359466</v>
-      </c>
-    </row>
-    <row r="9" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.473476303588299</v>
+      </c>
       <c r="E9">
         <v>1998</v>
       </c>
@@ -3669,23 +3691,27 @@
         <v>61.842077893741497</v>
       </c>
       <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4767123077626962</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>1.4767123077626962</v>
-      </c>
-      <c r="K9" s="2">
+        <v>1.0884326719451991</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7788738547998264E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6598300135323001</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>1.0884326719451991</v>
-      </c>
-      <c r="L9" s="2">
-        <f t="shared" si="0"/>
-        <v>5.7788738547998264E-2</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6598300135323001</v>
-      </c>
-    </row>
-    <row r="10" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.044741461732698</v>
+      </c>
       <c r="E10">
         <v>1999</v>
       </c>
@@ -3702,23 +3728,27 @@
         <v>61.4693003229279</v>
       </c>
       <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.44652655198269997</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>-0.44652655198269997</v>
-      </c>
-      <c r="K10" s="2">
+        <v>-0.1900935463796003</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.70554169824649904</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.37277757081359653</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>-0.1900935463796003</v>
-      </c>
-      <c r="L10" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.70554169824649904</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.37277757081359653</v>
-      </c>
-    </row>
-    <row r="11" spans="5:13" x14ac:dyDescent="0.25">
+        <v>63.687772878776627</v>
+      </c>
       <c r="E11">
         <v>2000</v>
       </c>
@@ -3735,23 +3765,27 @@
         <v>60.275093639639003</v>
       </c>
       <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2444669838610025</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>1.2444669838610025</v>
-      </c>
-      <c r="K11" s="2">
+        <v>-0.42531109689549851</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.0528235355009059</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.1942066832888969</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>-0.42531109689549851</v>
-      </c>
-      <c r="L11" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.0528235355009059</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.1942066832888969</v>
-      </c>
-    </row>
-    <row r="12" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.147221077506956</v>
+      </c>
       <c r="E12">
         <v>2001</v>
       </c>
@@ -3768,23 +3802,27 @@
         <v>61.674941518395102</v>
       </c>
       <c r="J12" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.71767385579290277</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
-        <v>-0.71767385579290277</v>
-      </c>
-      <c r="K12" s="2">
+        <v>0.61444078328010221</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.54117798867800104</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3998478787560984</v>
+      </c>
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.61444078328010221</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54117798867800104</v>
-      </c>
-      <c r="M12" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3998478787560984</v>
-      </c>
-    </row>
-    <row r="13" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.159145784015649</v>
+      </c>
       <c r="E13">
         <v>2002</v>
       </c>
@@ -3801,23 +3839,27 @@
         <v>60.798859888140001</v>
       </c>
       <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.26560387698409471</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
-        <v>-0.26560387698409471</v>
-      </c>
-      <c r="K13" s="2">
+        <v>0.64424612346618915</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.54513820980780281</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.87608163025510066</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>0.64424612346618915</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54513820980780281</v>
-      </c>
-      <c r="M13" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.87608163025510066</v>
-      </c>
-    </row>
-    <row r="14" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.279317020359571</v>
+      </c>
       <c r="E14">
         <v>2003</v>
       </c>
@@ -3834,23 +3876,27 @@
         <v>61.3824094235231</v>
       </c>
       <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>9.8158634572499182E-2</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="1"/>
-        <v>9.8158634572499182E-2</v>
-      </c>
-      <c r="K14" s="2">
+        <v>-0.36317600781779902</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16215278323790017</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.58354953538309928</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D15">
         <f t="shared" si="0"/>
-        <v>-0.36317600781779902</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16215278323790017</v>
-      </c>
-      <c r="M14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.58354953538309928</v>
-      </c>
-    </row>
-    <row r="15" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.235955481029023</v>
+      </c>
       <c r="E15">
         <v>2004</v>
       </c>
@@ -3867,23 +3913,27 @@
         <v>62.004777261934201</v>
       </c>
       <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.92737520845869881</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="1"/>
-        <v>0.92737520845869881</v>
-      </c>
-      <c r="K15" s="2">
+        <v>-1.4212239020099986</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.30196530218199769</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6223678384111011</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D16">
         <f t="shared" si="0"/>
-        <v>-1.4212239020099986</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.30196530218199769</v>
-      </c>
-      <c r="M15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6223678384111011</v>
-      </c>
-    </row>
-    <row r="16" spans="5:13" x14ac:dyDescent="0.25">
+        <v>64.5850641119969</v>
+      </c>
       <c r="E16">
         <v>2005</v>
       </c>
@@ -3900,23 +3950,27 @@
         <v>62.445541989067898</v>
       </c>
       <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.2234729689877</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="1"/>
-        <v>-1.2234729689877</v>
-      </c>
-      <c r="K16" s="2">
+        <v>1.7189601365007974</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46018262922469688</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.44076472713369697</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.7189601365007974</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.46018262922469688</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44076472713369697</v>
-      </c>
-    </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+        <v>64.690302885651789</v>
+      </c>
       <c r="E17">
         <v>2006</v>
       </c>
@@ -3933,23 +3987,27 @@
         <v>61.278345202734101</v>
       </c>
       <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2127003167889967</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="1"/>
-        <v>1.2127003167889967</v>
-      </c>
-      <c r="K17" s="2">
+        <v>0.21432569370109888</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16112587046330162</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.1671967863337969</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D18">
         <f t="shared" si="0"/>
-        <v>0.21432569370109888</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16112587046330162</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.1671967863337969</v>
-      </c>
-    </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+        <v>64.753292098406973</v>
+      </c>
       <c r="E18">
         <v>2007</v>
       </c>
@@ -3966,23 +4024,27 @@
         <v>62.025259689089403</v>
       </c>
       <c r="J18" s="2">
+        <f t="shared" si="2"/>
+        <v>0.29087163100380309</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="1"/>
-        <v>0.29087163100380309</v>
-      </c>
-      <c r="K18" s="2">
+        <v>-0.36881569326449437</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.41701357307390197</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.74691448635530122</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D19">
         <f t="shared" si="0"/>
-        <v>-0.36881569326449437</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.41701357307390197</v>
-      </c>
-      <c r="M18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.74691448635530122</v>
-      </c>
-    </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+        <v>64.097077648430044</v>
+      </c>
       <c r="E19">
         <v>2008</v>
       </c>
@@ -3999,23 +4061,27 @@
         <v>60.831270714207598</v>
       </c>
       <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.2687014703455972</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="1"/>
-        <v>-1.2687014703455972</v>
-      </c>
-      <c r="K19" s="2">
+        <v>-0.52769765677899727</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36553030209869775</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.1939889748818047</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D20">
         <f t="shared" si="0"/>
-        <v>-0.52769765677899727</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.36553030209869775</v>
-      </c>
-      <c r="M19" s="2">
-        <f t="shared" si="0"/>
-        <v>-1.1939889748818047</v>
-      </c>
-    </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+        <v>64.362145247566971</v>
+      </c>
       <c r="E20">
         <v>2009</v>
       </c>
@@ -4032,23 +4098,27 @@
         <v>61.494699837750098</v>
       </c>
       <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.53608726316989674</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="1"/>
-        <v>0.53608726316989674</v>
-      </c>
-      <c r="K20" s="2">
+        <v>-0.31884392578079712</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17959793561610127</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.66342912354249961</v>
+      </c>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D21">
         <f t="shared" si="0"/>
-        <v>-0.31884392578079712</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17959793561610127</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.66342912354249961</v>
-      </c>
-    </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+        <v>65.096803861565348</v>
+      </c>
       <c r="E21">
         <v>2010</v>
       </c>
@@ -4065,23 +4135,27 @@
         <v>61.989566978981998</v>
       </c>
       <c r="J21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.945387816888001</v>
+      </c>
+      <c r="K21" s="2">
         <f t="shared" si="1"/>
-        <v>0.945387816888001</v>
-      </c>
-      <c r="K21" s="2">
+        <v>1.5866149541843981</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.8235456310798099E-2</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49486714123190012</v>
+      </c>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D22">
         <f t="shared" si="0"/>
-        <v>1.5866149541843981</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="0"/>
-        <v>-8.8235456310798099E-2</v>
-      </c>
-      <c r="M21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.49486714123190012</v>
-      </c>
-    </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+        <v>64.917190311842035</v>
+      </c>
       <c r="E22">
         <v>2011</v>
       </c>
@@ -4098,23 +4172,27 @@
         <v>61.8748984034833</v>
       </c>
       <c r="J22" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.82830118614509729</v>
+      </c>
+      <c r="K22" s="2">
         <f t="shared" si="1"/>
-        <v>-0.82830118614509729</v>
-      </c>
-      <c r="K22" s="2">
+        <v>-0.12082019817650291</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.34533576092700002</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.11466857549869758</v>
+      </c>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D23">
         <f t="shared" si="0"/>
-        <v>-0.12082019817650291</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.34533576092700002</v>
-      </c>
-      <c r="M22" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.11466857549869758</v>
-      </c>
-    </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
+        <v>65.301739275584268</v>
+      </c>
       <c r="E23">
         <v>2012</v>
       </c>
@@ -4131,23 +4209,27 @@
         <v>61.2644168386907</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2490388460680961</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" ref="K23:K30" si="2">G23-G22</f>
+        <f t="shared" ref="K23:K30" si="3">G23-G22</f>
         <v>-1.8981846846003236E-2</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" ref="L23:L30" si="3">H23-H22</f>
+        <f t="shared" ref="L23:L30" si="4">H23-H22</f>
         <v>-8.1379579460502782E-2</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" ref="M23:M30" si="4">I23-I22</f>
+        <f t="shared" ref="M23:M30" si="5">I23-I22</f>
         <v>-0.6104815647926003</v>
       </c>
     </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>64.300986981960833</v>
+      </c>
       <c r="E24">
         <v>2013</v>
       </c>
@@ -4164,23 +4246,27 @@
         <v>61.315743848906202</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.4762692833056974</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.93501827893699385</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.35695137753339878</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.13270102155019E-2</v>
       </c>
     </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>64.612701463984706</v>
+      </c>
       <c r="E25">
         <v>2014</v>
       </c>
@@ -4197,19 +4283,19 @@
         <v>61.607502756968401</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69277635848320074</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.18571392198460046</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44803658353470155</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.2917589080621994</v>
       </c>
       <c r="N25" t="s">
@@ -4228,7 +4314,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>65.635512331914157</v>
+      </c>
       <c r="E26">
         <v>2015</v>
       </c>
@@ -4245,19 +4335,19 @@
         <v>63.418053393080903</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4177834139008993</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0257296004834018</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.16282017877900046</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8105506361125023</v>
       </c>
       <c r="O26">
@@ -4277,7 +4367,11 @@
         <v>8.6996536491236398E-2</v>
       </c>
     </row>
-    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>65.852710489289578</v>
+      </c>
       <c r="E27">
         <v>2016</v>
       </c>
@@ -4294,23 +4388,27 @@
         <v>63.590938149888302</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4919660138185975</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.57173347644850026</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.36779161757279866</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.17288475680739879</v>
       </c>
     </row>
-    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>65.452312997562274</v>
+      </c>
       <c r="E28">
         <v>2017</v>
       </c>
@@ -4327,23 +4425,27 @@
         <v>62.639196305907497</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.7936402919501973E-2</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.78029698306660578</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18838526305770387</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.95174184398080541</v>
       </c>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>65.047682853589649</v>
+      </c>
       <c r="E29">
         <v>2018</v>
       </c>
@@ -4360,23 +4462,27 @@
         <v>61.6572215968637</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.7429693324100981</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.69605216891079635</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.58962870334740103</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.98197470904379713</v>
       </c>
     </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>65.084283307324995</v>
+      </c>
       <c r="E30">
         <v>2019</v>
       </c>
@@ -4393,23 +4499,27 @@
         <v>62.0894082316251</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.78222665126499891</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.45828725658169844</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.95472908802669565</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.43218663476140051</v>
       </c>
     </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D31" s="3">
+        <f>D30-D6</f>
+        <v>1.1276931483524208</v>
+      </c>
       <c r="E31" t="s">
         <v>6</v>
       </c>
@@ -4418,19 +4528,23 @@
         <v>1.2332329525655013</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" ref="G31:H31" si="5">G30-G6</f>
+        <f t="shared" ref="G31:H31" si="6">G30-G6</f>
         <v>1.0911684624399953</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.17533411320819425</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" ref="I31" si="6">I30-I6</f>
+        <f t="shared" ref="I31" si="7">I30-I6</f>
         <v>2.0110370651959997</v>
       </c>
     </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f>MAX(D6:D30)-MIN(D6:D30)</f>
+        <v>2.8072426189247821</v>
+      </c>
       <c r="E32" t="s">
         <v>5</v>
       </c>
@@ -4439,11 +4553,11 @@
         <v>4.6109381953573987</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:I32" si="7">MAX(G6:G30)-MIN(G6:G30)</f>
+        <f t="shared" ref="G32:H32" si="8">MAX(G6:G30)-MIN(G6:G30)</f>
         <v>2.6414723395498072</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.6995093814796007</v>
       </c>
       <c r="I32" s="2">
@@ -4462,8 +4576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC960B77-A31D-4679-BF7E-2B47567D8405}">
   <dimension ref="B3:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5056,8 +5170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76788943-DE84-49BB-981C-A0946E7660AB}">
   <dimension ref="B3:P28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
arregla invierno y verano
</commit_message>
<xml_diff>
--- a/exel.xlsx
+++ b/exel.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Google Drive\Tareas\Patos\proyecto\daily_temp_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria José\Documents\9 semestre\Patos\proyecto\daily_temp_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC66D8A-6F85-45DB-AD41-3D5940D5DBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2580" windowWidth="24240" windowHeight="13290" activeTab="3" xr2:uid="{EB65F998-C7A7-4408-AC65-F4F555A00757}"/>
+    <workbookView xWindow="-24120" yWindow="2580" windowWidth="24240" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ciudades con mayor variacion'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -318,7 +317,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -401,6 +400,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -426,7 +426,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -679,82 +679,82 @@
             <c:numRef>
               <c:f>Hoja1!$G$6:$G$30</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>74.925373076021501</c:v>
+                  <c:v>73.494661115574104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.112963894586102</c:v>
+                  <c:v>72.430777049171098</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.970286244060603</c:v>
+                  <c:v>72.970619208715107</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.058718916005802</c:v>
+                  <c:v>74.411392071978597</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.868625369626201</c:v>
+                  <c:v>73.762325417041296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.443314272730703</c:v>
+                  <c:v>73.1592091798273</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75.057755056010805</c:v>
+                  <c:v>73.638130331959104</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.702001179476994</c:v>
+                  <c:v>74.4139540344853</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.338825171659195</c:v>
+                  <c:v>74.112700264265001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>73.917601269649197</c:v>
+                  <c:v>73.136822831793793</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>75.636561406149994</c:v>
+                  <c:v>74.703548532455102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>75.850887099851093</c:v>
+                  <c:v>74.075794562834602</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>75.482071406586599</c:v>
+                  <c:v>74.168548185996102</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>74.954373749807601</c:v>
+                  <c:v>73.465610415579704</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>74.635529824026804</c:v>
+                  <c:v>73.558727797268801</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>76.222144778211202</c:v>
+                  <c:v>74.833345027250402</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>76.101324580034699</c:v>
+                  <c:v>74.724123282321102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>76.082342733188696</c:v>
+                  <c:v>74.522597460774904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75.147324454251702</c:v>
+                  <c:v>73.983970723462306</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>74.961610532267102</c:v>
+                  <c:v>73.825856792270798</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>75.987340132750504</c:v>
+                  <c:v>75.068681773109702</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>76.559073609199004</c:v>
+                  <c:v>75.5429388476539</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>75.778776626132398</c:v>
+                  <c:v>74.526251818206106</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76.474828795043194</c:v>
+                  <c:v>75.308988053474494</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>76.016541538461496</c:v>
+                  <c:v>75.4107588776006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -802,82 +802,82 @@
             <c:numRef>
               <c:f>Hoja1!$H$6:$H$30</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>62.400744532340603</c:v>
+                  <c:v>47.028847128356198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.0914410058027</c:v>
+                  <c:v>44.573056739569701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.577145759268603</c:v>
+                  <c:v>46.831556366153897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61.634934497816602</c:v>
+                  <c:v>47.797942232616101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.929392799570103</c:v>
+                  <c:v>47.444269954327602</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59.876569264069197</c:v>
+                  <c:v>47.578728797760199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.417747252747198</c:v>
+                  <c:v>46.385611072800003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.962885462555001</c:v>
+                  <c:v>48.102629715870599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61.125038245792901</c:v>
+                  <c:v>45.6908247446855</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60.823072943610903</c:v>
+                  <c:v>46.717186393473902</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61.2832555728356</c:v>
+                  <c:v>46.913355876478597</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61.444381443298902</c:v>
+                  <c:v>48.138775711292197</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>61.027367870225</c:v>
+                  <c:v>47.734886236470203</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>61.392898172323697</c:v>
+                  <c:v>46.663119931724999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>61.572496107939799</c:v>
+                  <c:v>46.835541174070698</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>61.484260651629</c:v>
+                  <c:v>46.6650386551105</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>61.829596412556</c:v>
+                  <c:v>46.407577572239703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>61.748216833095498</c:v>
+                  <c:v>49.4585445128915</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>62.105168210628896</c:v>
+                  <c:v>46.835843539743998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>62.553204794163598</c:v>
+                  <c:v>45.492982064894598</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>62.390384615384598</c:v>
+                  <c:v>46.774414167854196</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>62.022592997811799</c:v>
+                  <c:v>49.587242217963599</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>62.210978260869503</c:v>
+                  <c:v>49.822213721746998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>61.621349557522102</c:v>
+                  <c:v>47.645999381206401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>62.576078645548797</c:v>
+                  <c:v>47.395260469318899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1065,7 +1065,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1989842288"/>
@@ -1126,7 +1126,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1989863088"/>
@@ -1143,6 +1143,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1168,12 +1169,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1181,7 +1183,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1205,7 +1206,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2048,7 +2049,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1276656944"/>
@@ -2107,7 +2108,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="764534608"/>
@@ -2124,6 +2125,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2131,7 +2133,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2155,7 +2156,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3751,7 +3752,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1513614623"/>
@@ -3811,7 +3812,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1513613375"/>
@@ -3856,7 +3857,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3872,7 +3873,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4189,7 +4190,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1276068416"/>
@@ -4248,7 +4249,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1276067168"/>
@@ -4265,6 +4266,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4272,7 +4274,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4296,7 +4297,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4347,7 +4348,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4444,7 +4445,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:strRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -4452,7 +4453,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:strRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -4515,7 +4516,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1326741456"/>
@@ -4574,7 +4575,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1326738960"/>
@@ -4591,6 +4592,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4598,7 +4600,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4622,7 +4623,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4648,6 +4649,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4673,7 +4675,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4894,7 +4896,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1399627936"/>
@@ -4953,7 +4955,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1399627520"/>
@@ -4970,6 +4972,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4977,7 +4980,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5001,7 +5003,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7777,9 +7779,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8298,11 +8300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C714A26-8582-4DED-B929-AA40AE456B7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8346,7 +8348,7 @@
     <row r="6" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>SUM(F6:I6)/4</f>
-        <v>63.956590158972574</v>
+        <v>59.755937817864627</v>
       </c>
       <c r="E6">
         <v>1995</v>
@@ -8354,11 +8356,11 @@
       <c r="F6" s="2">
         <v>58.421871861099099</v>
       </c>
-      <c r="G6" s="2">
-        <v>74.925373076021501</v>
-      </c>
-      <c r="H6" s="2">
-        <v>62.400744532340603</v>
+      <c r="G6">
+        <v>73.494661115574104</v>
+      </c>
+      <c r="H6">
+        <v>47.028847128356198</v>
       </c>
       <c r="I6" s="2">
         <v>60.0783711664291</v>
@@ -8369,7 +8371,7 @@
     <row r="7" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D7">
         <f>SUM(F7:I7)/4</f>
-        <v>63.045467870364796</v>
+        <v>58.495325092452795</v>
       </c>
       <c r="E7">
         <v>1996</v>
@@ -8377,11 +8379,11 @@
       <c r="F7" s="2">
         <v>57.5010425020048</v>
       </c>
-      <c r="G7" s="2">
-        <v>74.112963894586102</v>
-      </c>
-      <c r="H7" s="2">
-        <v>61.0914410058027</v>
+      <c r="G7">
+        <v>72.430777049171098</v>
+      </c>
+      <c r="H7">
+        <v>44.573056739569701</v>
       </c>
       <c r="I7" s="2">
         <v>59.476424079065602</v>
@@ -8392,11 +8394,11 @@
       </c>
       <c r="K7" s="2">
         <f t="shared" ref="K7:M22" si="0">G7-G6</f>
-        <v>-0.81240918143539886</v>
+        <v>-1.0638840664030056</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="0"/>
-        <v>-1.3093035265379029</v>
+        <v>-2.4557903887864967</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="0"/>
@@ -8405,8 +8407,8 @@
     </row>
     <row r="8" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D8">
-        <f t="shared" ref="D7:D30" si="1">SUM(F8:I8)/4</f>
-        <v>63.402785370641247</v>
+        <f t="shared" ref="D8:D30" si="1">SUM(F8:I8)/4</f>
+        <v>59.466471263526202</v>
       </c>
       <c r="E8">
         <v>1997</v>
@@ -8414,11 +8416,11 @@
       <c r="F8" s="2">
         <v>57.881461599026601</v>
       </c>
-      <c r="G8" s="2">
-        <v>73.970286244060603</v>
-      </c>
-      <c r="H8" s="2">
-        <v>61.577145759268603</v>
+      <c r="G8">
+        <v>72.970619208715107</v>
+      </c>
+      <c r="H8">
+        <v>46.831556366153897</v>
       </c>
       <c r="I8" s="2">
         <v>60.182247880209196</v>
@@ -8429,11 +8431,11 @@
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>-0.14267765052549919</v>
+        <v>0.53984215954400838</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>0.48570475346590314</v>
+        <v>2.2584996265841966</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="0"/>
@@ -8443,7 +8445,7 @@
     <row r="9" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>64.473476303588299</v>
+        <v>60.852396526281375</v>
       </c>
       <c r="E9">
         <v>1998</v>
@@ -8451,11 +8453,11 @@
       <c r="F9" s="2">
         <v>59.358173906789297</v>
       </c>
-      <c r="G9" s="2">
-        <v>75.058718916005802</v>
-      </c>
-      <c r="H9" s="2">
-        <v>61.634934497816602</v>
+      <c r="G9">
+        <v>74.411392071978597</v>
+      </c>
+      <c r="H9">
+        <v>47.797942232616101</v>
       </c>
       <c r="I9" s="2">
         <v>61.842077893741497</v>
@@ -8466,11 +8468,11 @@
       </c>
       <c r="K9" s="2">
         <f t="shared" si="0"/>
-        <v>1.0884326719451991</v>
+        <v>1.44077286326349</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" si="0"/>
-        <v>5.7788738547998264E-2</v>
+        <v>0.96638586646220404</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="0"/>
@@ -8480,7 +8482,7 @@
     <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>64.044741461732698</v>
+        <v>60.396885762275851</v>
       </c>
       <c r="E10">
         <v>1999</v>
@@ -8488,11 +8490,11 @@
       <c r="F10" s="2">
         <v>58.911647354806597</v>
       </c>
-      <c r="G10" s="2">
-        <v>74.868625369626201</v>
-      </c>
-      <c r="H10" s="2">
-        <v>60.929392799570103</v>
+      <c r="G10">
+        <v>73.762325417041296</v>
+      </c>
+      <c r="H10">
+        <v>47.444269954327602</v>
       </c>
       <c r="I10" s="2">
         <v>61.4693003229279</v>
@@ -8503,11 +8505,11 @@
       </c>
       <c r="K10" s="2">
         <f t="shared" si="0"/>
-        <v>-0.1900935463796003</v>
+        <v>-0.64906665493730031</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="0"/>
-        <v>-0.70554169824649904</v>
+        <v>-0.35367227828849934</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="0"/>
@@ -8517,7 +8519,7 @@
     <row r="11" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>63.687772878776627</v>
+        <v>60.292286488973524</v>
       </c>
       <c r="E11">
         <v>2000</v>
@@ -8525,11 +8527,11 @@
       <c r="F11" s="2">
         <v>60.156114338667599</v>
       </c>
-      <c r="G11" s="2">
-        <v>74.443314272730703</v>
-      </c>
-      <c r="H11" s="2">
-        <v>59.876569264069197</v>
+      <c r="G11">
+        <v>73.1592091798273</v>
+      </c>
+      <c r="H11">
+        <v>47.578728797760199</v>
       </c>
       <c r="I11" s="2">
         <v>60.275093639639003</v>
@@ -8540,11 +8542,11 @@
       </c>
       <c r="K11" s="2">
         <f t="shared" si="0"/>
-        <v>-0.42531109689549851</v>
+        <v>-0.60311623721399599</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="0"/>
-        <v>-1.0528235355009059</v>
+        <v>0.13445884343259706</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="0"/>
@@ -8554,7 +8556,7 @@
     <row r="12" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>64.147221077506956</v>
+        <v>60.284280851507233</v>
       </c>
       <c r="E12">
         <v>2001</v>
@@ -8562,11 +8564,11 @@
       <c r="F12" s="2">
         <v>59.438440482874697</v>
       </c>
-      <c r="G12" s="2">
-        <v>75.057755056010805</v>
-      </c>
-      <c r="H12" s="2">
-        <v>60.417747252747198</v>
+      <c r="G12">
+        <v>73.638130331959104</v>
+      </c>
+      <c r="H12">
+        <v>46.385611072800003</v>
       </c>
       <c r="I12" s="2">
         <v>61.674941518395102</v>
@@ -8577,11 +8579,11 @@
       </c>
       <c r="K12" s="2">
         <f t="shared" si="0"/>
-        <v>0.61444078328010221</v>
+        <v>0.47892115213180375</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" si="0"/>
-        <v>0.54117798867800104</v>
+        <v>-1.1931177249601959</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="0"/>
@@ -8591,7 +8593,7 @@
     <row r="13" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>64.159145784015649</v>
+        <v>60.622070061096622</v>
       </c>
       <c r="E13">
         <v>2002</v>
@@ -8599,11 +8601,11 @@
       <c r="F13" s="2">
         <v>59.172836605890602</v>
       </c>
-      <c r="G13" s="2">
-        <v>75.702001179476994</v>
-      </c>
-      <c r="H13" s="2">
-        <v>60.962885462555001</v>
+      <c r="G13">
+        <v>74.4139540344853</v>
+      </c>
+      <c r="H13">
+        <v>48.102629715870599</v>
       </c>
       <c r="I13" s="2">
         <v>60.798859888140001</v>
@@ -8614,11 +8616,11 @@
       </c>
       <c r="K13" s="2">
         <f t="shared" si="0"/>
-        <v>0.64424612346618915</v>
+        <v>0.77582370252619626</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="0"/>
-        <v>0.54513820980780281</v>
+        <v>1.7170186430705954</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="0"/>
@@ -8628,7 +8630,7 @@
     <row r="14" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>64.279317020359571</v>
+        <v>60.114232418234181</v>
       </c>
       <c r="E14">
         <v>2003</v>
@@ -8636,11 +8638,11 @@
       <c r="F14" s="2">
         <v>59.270995240463101</v>
       </c>
-      <c r="G14" s="2">
-        <v>75.338825171659195</v>
-      </c>
-      <c r="H14" s="2">
-        <v>61.125038245792901</v>
+      <c r="G14">
+        <v>74.112700264265001</v>
+      </c>
+      <c r="H14">
+        <v>45.6908247446855</v>
       </c>
       <c r="I14" s="2">
         <v>61.3824094235231</v>
@@ -8651,11 +8653,11 @@
       </c>
       <c r="K14" s="2">
         <f t="shared" si="0"/>
-        <v>-0.36317600781779902</v>
+        <v>-0.30125377022029909</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="0"/>
-        <v>0.16215278323790017</v>
+        <v>-2.4118049711850986</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="0"/>
@@ -8665,7 +8667,7 @@
     <row r="15" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>64.235955481029023</v>
+        <v>60.514289234030926</v>
       </c>
       <c r="E15">
         <v>2004</v>
@@ -8673,11 +8675,11 @@
       <c r="F15" s="2">
         <v>60.1983704489218</v>
       </c>
-      <c r="G15" s="2">
-        <v>73.917601269649197</v>
-      </c>
-      <c r="H15" s="2">
-        <v>60.823072943610903</v>
+      <c r="G15">
+        <v>73.136822831793793</v>
+      </c>
+      <c r="H15">
+        <v>46.717186393473902</v>
       </c>
       <c r="I15" s="2">
         <v>62.004777261934201</v>
@@ -8688,11 +8690,11 @@
       </c>
       <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>-1.4212239020099986</v>
+        <v>-0.97587743247120784</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="0"/>
-        <v>-0.30196530218199769</v>
+        <v>1.0263616487884022</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="0"/>
@@ -8702,7 +8704,7 @@
     <row r="16" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>64.5850641119969</v>
+        <v>60.759335969483921</v>
       </c>
       <c r="E16">
         <v>2005</v>
@@ -8710,11 +8712,11 @@
       <c r="F16" s="2">
         <v>58.9748974799341</v>
       </c>
-      <c r="G16" s="2">
-        <v>75.636561406149994</v>
-      </c>
-      <c r="H16" s="2">
-        <v>61.2832555728356</v>
+      <c r="G16">
+        <v>74.703548532455102</v>
+      </c>
+      <c r="H16">
+        <v>46.913355876478597</v>
       </c>
       <c r="I16" s="2">
         <v>62.445541989067898</v>
@@ -8725,11 +8727,11 @@
       </c>
       <c r="K16" s="2">
         <f t="shared" si="0"/>
-        <v>1.7189601365007974</v>
+        <v>1.5667257006613085</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="0"/>
-        <v>0.46018262922469688</v>
+        <v>0.19616948300469517</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="0"/>
@@ -8739,7 +8741,7 @@
     <row r="17" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>64.690302885651789</v>
+        <v>60.920128318396003</v>
       </c>
       <c r="E17">
         <v>2006</v>
@@ -8747,11 +8749,11 @@
       <c r="F17" s="2">
         <v>60.187597796723097</v>
       </c>
-      <c r="G17" s="2">
-        <v>75.850887099851093</v>
-      </c>
-      <c r="H17" s="2">
-        <v>61.444381443298902</v>
+      <c r="G17">
+        <v>74.075794562834602</v>
+      </c>
+      <c r="H17">
+        <v>48.138775711292197</v>
       </c>
       <c r="I17" s="2">
         <v>61.278345202734101</v>
@@ -8762,11 +8764,11 @@
       </c>
       <c r="K17" s="2">
         <f t="shared" si="0"/>
-        <v>0.21432569370109888</v>
+        <v>-0.62775396962049967</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="0"/>
-        <v>0.16112587046330162</v>
+        <v>1.2254198348136001</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="0"/>
@@ -8776,7 +8778,7 @@
     <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>64.753292098406973</v>
+        <v>61.101790884820652</v>
       </c>
       <c r="E18">
         <v>2007</v>
@@ -8784,11 +8786,11 @@
       <c r="F18" s="2">
         <v>60.4784694277269</v>
       </c>
-      <c r="G18" s="2">
-        <v>75.482071406586599</v>
-      </c>
-      <c r="H18" s="2">
-        <v>61.027367870225</v>
+      <c r="G18">
+        <v>74.168548185996102</v>
+      </c>
+      <c r="H18">
+        <v>47.734886236470203</v>
       </c>
       <c r="I18" s="2">
         <v>62.025259689089403</v>
@@ -8799,11 +8801,11 @@
       </c>
       <c r="K18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.36881569326449437</v>
+        <v>9.2753623161499377E-2</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.41701357307390197</v>
+        <v>-0.40388947482199455</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="0"/>
@@ -8813,7 +8815,7 @@
     <row r="19" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>64.097077648430044</v>
+        <v>60.042442254723397</v>
       </c>
       <c r="E19">
         <v>2008</v>
@@ -8821,11 +8823,11 @@
       <c r="F19" s="2">
         <v>59.209767957381302</v>
       </c>
-      <c r="G19" s="2">
-        <v>74.954373749807601</v>
-      </c>
-      <c r="H19" s="2">
-        <v>61.392898172323697</v>
+      <c r="G19">
+        <v>73.465610415579704</v>
+      </c>
+      <c r="H19">
+        <v>46.663119931724999</v>
       </c>
       <c r="I19" s="2">
         <v>60.831270714207598</v>
@@ -8836,11 +8838,11 @@
       </c>
       <c r="K19" s="2">
         <f t="shared" si="0"/>
-        <v>-0.52769765677899727</v>
+        <v>-0.70293777041639771</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="0"/>
-        <v>0.36553030209869775</v>
+        <v>-1.0717663047452035</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="0"/>
@@ -8850,7 +8852,7 @@
     <row r="20" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>64.362145247566971</v>
+        <v>60.408706007410196</v>
       </c>
       <c r="E20">
         <v>2009</v>
@@ -8858,11 +8860,11 @@
       <c r="F20" s="2">
         <v>59.745855220551199</v>
       </c>
-      <c r="G20" s="2">
-        <v>74.635529824026804</v>
-      </c>
-      <c r="H20" s="2">
-        <v>61.572496107939799</v>
+      <c r="G20">
+        <v>73.558727797268801</v>
+      </c>
+      <c r="H20">
+        <v>46.835541174070698</v>
       </c>
       <c r="I20" s="2">
         <v>61.494699837750098</v>
@@ -8873,11 +8875,11 @@
       </c>
       <c r="K20" s="2">
         <f t="shared" si="0"/>
-        <v>-0.31884392578079712</v>
+        <v>9.3117381689097556E-2</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="0"/>
-        <v>0.17959793561610127</v>
+        <v>0.172421242345699</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="0"/>
@@ -8887,7 +8889,7 @@
     <row r="21" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>65.096803861565348</v>
+        <v>61.044798424695522</v>
       </c>
       <c r="E21">
         <v>2010</v>
@@ -8895,11 +8897,11 @@
       <c r="F21" s="2">
         <v>60.6912430374392</v>
       </c>
-      <c r="G21" s="2">
-        <v>76.222144778211202</v>
-      </c>
-      <c r="H21" s="2">
-        <v>61.484260651629</v>
+      <c r="G21">
+        <v>74.833345027250402</v>
+      </c>
+      <c r="H21">
+        <v>46.6650386551105</v>
       </c>
       <c r="I21" s="2">
         <v>61.989566978981998</v>
@@ -8910,11 +8912,11 @@
       </c>
       <c r="K21" s="2">
         <f t="shared" si="0"/>
-        <v>1.5866149541843981</v>
+        <v>1.274617229981601</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="0"/>
-        <v>-8.8235456310798099E-2</v>
+        <v>-0.1705025189601983</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="0"/>
@@ -8924,7 +8926,7 @@
     <row r="22" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>64.917190311842035</v>
+        <v>60.717385277334557</v>
       </c>
       <c r="E22">
         <v>2011</v>
@@ -8932,11 +8934,11 @@
       <c r="F22" s="2">
         <v>59.862941851294103</v>
       </c>
-      <c r="G22" s="2">
-        <v>76.101324580034699</v>
-      </c>
-      <c r="H22" s="2">
-        <v>61.829596412556</v>
+      <c r="G22">
+        <v>74.724123282321102</v>
+      </c>
+      <c r="H22">
+        <v>46.407577572239703</v>
       </c>
       <c r="I22" s="2">
         <v>61.8748984034833</v>
@@ -8947,11 +8949,11 @@
       </c>
       <c r="K22" s="2">
         <f t="shared" si="0"/>
-        <v>-0.12082019817650291</v>
+        <v>-0.10922174492930026</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="0"/>
-        <v>0.34533576092700002</v>
+        <v>-0.2574610828707975</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="0"/>
@@ -8961,7 +8963,7 @@
     <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>65.301739275584268</v>
+        <v>61.839384877429829</v>
       </c>
       <c r="E23">
         <v>2012</v>
@@ -8969,11 +8971,11 @@
       <c r="F23" s="2">
         <v>62.111980697362199</v>
       </c>
-      <c r="G23" s="2">
-        <v>76.082342733188696</v>
-      </c>
-      <c r="H23" s="2">
-        <v>61.748216833095498</v>
+      <c r="G23">
+        <v>74.522597460774904</v>
+      </c>
+      <c r="H23">
+        <v>49.4585445128915</v>
       </c>
       <c r="I23" s="2">
         <v>61.2644168386907</v>
@@ -8984,11 +8986,11 @@
       </c>
       <c r="K23" s="2">
         <f t="shared" ref="K23:K30" si="3">G23-G22</f>
-        <v>-1.8981846846003236E-2</v>
+        <v>-0.20152582154619836</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" ref="L23:L30" si="4">H23-H22</f>
-        <v>-8.1379579460502782E-2</v>
+        <v>3.0509669406517972</v>
       </c>
       <c r="M23" s="2">
         <f t="shared" ref="M23:M30" si="5">I23-I22</f>
@@ -8998,7 +9000,7 @@
     <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>64.300986981960833</v>
+        <v>60.192817381542248</v>
       </c>
       <c r="E24">
         <v>2013</v>
@@ -9006,11 +9008,11 @@
       <c r="F24" s="2">
         <v>58.635711414056502</v>
       </c>
-      <c r="G24" s="2">
-        <v>75.147324454251702</v>
-      </c>
-      <c r="H24" s="2">
-        <v>62.105168210628896</v>
+      <c r="G24">
+        <v>73.983970723462306</v>
+      </c>
+      <c r="H24">
+        <v>46.835843539743998</v>
       </c>
       <c r="I24" s="2">
         <v>61.315743848906202</v>
@@ -9021,11 +9023,11 @@
       </c>
       <c r="K24" s="2">
         <f t="shared" si="3"/>
-        <v>-0.93501827893699385</v>
+        <v>-0.53862673731259747</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="4"/>
-        <v>0.35695137753339878</v>
+        <v>-2.6227009731475022</v>
       </c>
       <c r="M24" s="2">
         <f t="shared" si="5"/>
@@ -9035,7 +9037,7 @@
     <row r="25" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>64.612701463984706</v>
+        <v>60.06370734666838</v>
       </c>
       <c r="E25">
         <v>2014</v>
@@ -9043,11 +9045,11 @@
       <c r="F25" s="2">
         <v>59.328487772539702</v>
       </c>
-      <c r="G25" s="2">
-        <v>74.961610532267102</v>
-      </c>
-      <c r="H25" s="2">
-        <v>62.553204794163598</v>
+      <c r="G25">
+        <v>73.825856792270798</v>
+      </c>
+      <c r="H25">
+        <v>45.492982064894598</v>
       </c>
       <c r="I25" s="2">
         <v>61.607502756968401</v>
@@ -9058,11 +9060,11 @@
       </c>
       <c r="K25" s="2">
         <f t="shared" si="3"/>
-        <v>-0.18571392198460046</v>
+        <v>-0.15811393119150807</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="4"/>
-        <v>0.44803658353470155</v>
+        <v>-1.3428614748493999</v>
       </c>
       <c r="M25" s="2">
         <f t="shared" si="5"/>
@@ -9087,7 +9089,7 @@
     <row r="26" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>65.635512331914157</v>
+        <v>61.501855130121349</v>
       </c>
       <c r="E26">
         <v>2015</v>
@@ -9095,11 +9097,11 @@
       <c r="F26" s="2">
         <v>60.746271186440602</v>
       </c>
-      <c r="G26" s="2">
-        <v>75.987340132750504</v>
-      </c>
-      <c r="H26" s="2">
-        <v>62.390384615384598</v>
+      <c r="G26">
+        <v>75.068681773109702</v>
+      </c>
+      <c r="H26">
+        <v>46.774414167854196</v>
       </c>
       <c r="I26" s="2">
         <v>63.418053393080903</v>
@@ -9110,11 +9112,11 @@
       </c>
       <c r="K26" s="2">
         <f t="shared" si="3"/>
-        <v>1.0257296004834018</v>
+        <v>1.242824980838904</v>
       </c>
       <c r="L26" s="2">
         <f t="shared" si="4"/>
-        <v>-0.16282017877900046</v>
+        <v>1.2814321029595988</v>
       </c>
       <c r="M26" s="2">
         <f t="shared" si="5"/>
@@ -9126,11 +9128,11 @@
       </c>
       <c r="P26">
         <f>SLOPE(G6:G30,$E$6:$E$30)</f>
-        <v>7.1341999414166149E-2</v>
+        <v>7.904985994209901E-2</v>
       </c>
       <c r="Q26">
         <f>SLOPE(H6:H30,$E$6:$E$30)</f>
-        <v>5.197278028529758E-2</v>
+        <v>5.7546754499446337E-2</v>
       </c>
       <c r="R26">
         <f>SLOPE(I6:I30,$E$6:$E$30)</f>
@@ -9140,7 +9142,7 @@
     <row r="27" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>65.852710489289578</v>
+        <v>62.48983910394125</v>
       </c>
       <c r="E27">
         <v>2016</v>
@@ -9148,11 +9150,11 @@
       <c r="F27" s="2">
         <v>61.238237200259199</v>
       </c>
-      <c r="G27" s="2">
-        <v>76.559073609199004</v>
-      </c>
-      <c r="H27" s="2">
-        <v>62.022592997811799</v>
+      <c r="G27">
+        <v>75.5429388476539</v>
+      </c>
+      <c r="H27">
+        <v>49.587242217963599</v>
       </c>
       <c r="I27" s="2">
         <v>63.590938149888302</v>
@@ -9163,11 +9165,11 @@
       </c>
       <c r="K27" s="2">
         <f t="shared" si="3"/>
-        <v>0.57173347644850026</v>
+        <v>0.47425707454419808</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" si="4"/>
-        <v>-0.36779161757279866</v>
+        <v>2.8128280501094025</v>
       </c>
       <c r="M27" s="2">
         <f t="shared" si="5"/>
@@ -9177,7 +9179,7 @@
     <row r="28" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>65.452312997562274</v>
+        <v>62.041990660800074</v>
       </c>
       <c r="E28">
         <v>2017</v>
@@ -9185,11 +9187,11 @@
       <c r="F28" s="2">
         <v>61.180300797339697</v>
       </c>
-      <c r="G28" s="2">
-        <v>75.778776626132398</v>
-      </c>
-      <c r="H28" s="2">
-        <v>62.210978260869503</v>
+      <c r="G28">
+        <v>74.526251818206106</v>
+      </c>
+      <c r="H28">
+        <v>49.822213721746998</v>
       </c>
       <c r="I28" s="2">
         <v>62.639196305907497</v>
@@ -9200,11 +9202,11 @@
       </c>
       <c r="K28" s="2">
         <f t="shared" si="3"/>
-        <v>-0.78029698306660578</v>
+        <v>-1.0166870294477945</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" si="4"/>
-        <v>0.18838526305770387</v>
+        <v>0.23497150378339882</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" si="5"/>
@@ -9214,7 +9216,7 @@
     <row r="29" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>65.047682853589649</v>
+        <v>61.262385124118552</v>
       </c>
       <c r="E29">
         <v>2018</v>
@@ -9222,11 +9224,11 @@
       <c r="F29" s="2">
         <v>60.437331464929599</v>
       </c>
-      <c r="G29" s="2">
-        <v>76.474828795043194</v>
-      </c>
-      <c r="H29" s="2">
-        <v>61.621349557522102</v>
+      <c r="G29">
+        <v>75.308988053474494</v>
+      </c>
+      <c r="H29">
+        <v>47.645999381206401</v>
       </c>
       <c r="I29" s="2">
         <v>61.6572215968637</v>
@@ -9237,11 +9239,11 @@
       </c>
       <c r="K29" s="2">
         <f t="shared" si="3"/>
-        <v>0.69605216891079635</v>
+        <v>0.78273623526838776</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" si="4"/>
-        <v>-0.58962870334740103</v>
+        <v>-2.1762143405405965</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="5"/>
@@ -9251,7 +9253,7 @@
     <row r="30" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D30">
         <f t="shared" si="1"/>
-        <v>65.084283307324995</v>
+        <v>61.137633098052305</v>
       </c>
       <c r="E30">
         <v>2019</v>
@@ -9259,11 +9261,11 @@
       <c r="F30" s="2">
         <v>59.6551048136646</v>
       </c>
-      <c r="G30" s="2">
-        <v>76.016541538461496</v>
-      </c>
-      <c r="H30" s="2">
-        <v>62.576078645548797</v>
+      <c r="G30">
+        <v>75.4107588776006</v>
+      </c>
+      <c r="H30">
+        <v>47.395260469318899</v>
       </c>
       <c r="I30" s="2">
         <v>62.0894082316251</v>
@@ -9274,11 +9276,11 @@
       </c>
       <c r="K30" s="2">
         <f t="shared" si="3"/>
-        <v>-0.45828725658169844</v>
+        <v>0.10177082412610616</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" si="4"/>
-        <v>0.95472908802669565</v>
+        <v>-0.25073891188750252</v>
       </c>
       <c r="M30" s="2">
         <f t="shared" si="5"/>
@@ -9288,7 +9290,7 @@
     <row r="31" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <f>D30-D6</f>
-        <v>1.1276931483524208</v>
+        <v>1.3816952801876781</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -9297,23 +9299,21 @@
         <f>F30-F6</f>
         <v>1.2332329525655013</v>
       </c>
-      <c r="G31" s="3">
-        <f t="shared" ref="G31:H31" si="6">G30-G6</f>
-        <v>1.0911684624399953</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="6"/>
-        <v>0.17533411320819425</v>
+      <c r="G31">
+        <v>73.191208772344893</v>
+      </c>
+      <c r="H31">
+        <v>49.034296844208797</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" ref="I31" si="7">I30-I6</f>
+        <f t="shared" ref="I31" si="6">I30-I6</f>
         <v>2.0110370651959997</v>
       </c>
     </row>
     <row r="32" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f>MAX(D6:D30)-MIN(D6:D30)</f>
-        <v>2.8072426189247821</v>
+        <v>3.9945140114884552</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -9323,12 +9323,12 @@
         <v>4.6109381953573987</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:H32" si="8">MAX(G6:G30)-MIN(G6:G30)</f>
-        <v>2.6414723395498072</v>
+        <f t="shared" ref="G32:H32" si="7">MAX(G6:G30)-MIN(G6:G30)</f>
+        <v>3.1121617984828021</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="8"/>
-        <v>2.6995093814796007</v>
+        <f t="shared" si="7"/>
+        <v>5.249156982177297</v>
       </c>
       <c r="I32" s="2">
         <f>MAX(I6:I30)-MIN(I6:I30)</f>
@@ -9343,7 +9343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC960B77-A31D-4679-BF7E-2B47567D8405}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N107"/>
   <sheetViews>
     <sheetView topLeftCell="B82" workbookViewId="0">
@@ -11214,7 +11214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76788943-DE84-49BB-981C-A0946E7660AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P56"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -12350,7 +12350,7 @@
         <v>2010</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:H47" si="17">(C19-32)*(5/9)</f>
+        <f t="shared" ref="C47:G47" si="17">(C19-32)*(5/9)</f>
         <v>27.291389781519836</v>
       </c>
       <c r="D47">
@@ -12693,10 +12693,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C264258-D332-44C4-B410-5AB85B8FE2DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>

</xml_diff>